<commit_message>
don't run the tests when importing the test module in download_with_timer.py
</commit_message>
<xml_diff>
--- a/test/sheets/output.xlsx
+++ b/test/sheets/output.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Timeout should only count from when we start trying for that file in particular
</commit_message>
<xml_diff>
--- a/test/sheets/output.xlsx
+++ b/test/sheets/output.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">

</xml_diff>